<commit_message>
commiting for pulling without errors <(｀^´)>
</commit_message>
<xml_diff>
--- a/alu-4/testvektoren.xlsx
+++ b/alu-4/testvektoren.xlsx
@@ -618,7 +618,7 @@
   <dimension ref="A1:AH31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
         <v>32</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>32</v>
@@ -1365,7 +1365,7 @@
         <v>32</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>32</v>
@@ -2034,7 +2034,7 @@
         <v>32</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X16" s="1" t="s">
         <v>32</v>
@@ -2469,7 +2469,7 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="K3:S3 H3:I3 D3 G3 J3 E3:F3 D4:T4 D6:T6 D5:T5 AB5:AE5 Y5 V5 U4:AG4 V3:AF3 U6:V8 U3 AG3 U5 Z5:AA5 AF5:AG5 D7:S8 T11 D10:AG10 D11:S11 U11:AG11 D9:V9 Y9:AG9 Y6:AG8 X9 W6:X8 W5:X5 W9 D12:AG13" numberStoredAsText="1"/>
+    <ignoredError sqref="K3:S3 H3:I3 D3 G3 J3 E3:F3 D4:T4 D6:T6 D5:T5 AB5:AE5 Y5 V5 U4:AG4 V3:AF3 U6:V8 U3 AG3 U5 Z5:AA5 AF5:AG5 D7:S8 T11 D10:V10 D11:S11 U11:V11 D9:V9 Y9:AG9 Y6:AG8 X9 W6:X8 X5 D13:V13 X10:AG10 X11:AG11 D12:V12 X12:AG12 X13:AG13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>